<commit_message>
Adding Master Data XLS
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-app_detail.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-app_detail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -124,6 +124,45 @@
   </si>
   <si>
     <t>البوابة الإلكترونية لخدمات إنشاء معرف المشاركة</t>
+  </si>
+  <si>
+    <t>Pré-inscription</t>
+  </si>
+  <si>
+    <t>Portail Web pour les pré-inscriptions</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>Client dinscription</t>
+  </si>
+  <si>
+    <t>Application de bureau pour les inscriptions</t>
+  </si>
+  <si>
+    <t>Processeur dinscription</t>
+  </si>
+  <si>
+    <t>Demande de post-inscription</t>
+  </si>
+  <si>
+    <t>Authentification ID</t>
+  </si>
+  <si>
+    <t>Application pour lauthentification du fournisseur de services tiers</t>
+  </si>
+  <si>
+    <t>Contrôle didentité</t>
+  </si>
+  <si>
+    <t>Portail Web pour la configuration dapplications</t>
+  </si>
+  <si>
+    <t>Portail Résident</t>
+  </si>
+  <si>
+    <t>Portail Web pour les services de génération de post-ID</t>
   </si>
 </sst>
 </file>
@@ -964,11 +1003,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1269,7 +1314,146 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>10013</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>10014</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>10015</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>10016</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>10017</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>10018</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>